<commit_message>
added missing nature and reporting type
</commit_message>
<xml_diff>
--- a/source_data/QuaL_2_data.xlsx
+++ b/source_data/QuaL_2_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gender_data_portal\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFEEB00-6F5D-405C-B382-0FFD0445329F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE762312-3CE5-4DBF-BB3A-C18A4C1CFF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="2a - Whether or not ratified IL" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2a - Whether or not ratified IL'!$A$1:$Q$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2a - Whether or not ratified IL'!$A$1:$U$106</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="192">
   <si>
     <t>Whether or not ratified ILO convention 156 on workers with familiy responsibilities</t>
   </si>
@@ -585,6 +585,30 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>NATURE</t>
+  </si>
+  <si>
+    <t>NATURE_DESC</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Country Data</t>
+  </si>
+  <si>
+    <t>REPORTING_TYPE</t>
+  </si>
+  <si>
+    <t>REPORTING_TYPE_DESC</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Global</t>
   </si>
 </sst>
 </file>
@@ -1435,11 +1459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q106"/>
+  <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,10 +1482,14 @@
     <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>175</v>
       </c>
@@ -1508,13 +1536,25 @@
         <v>146</v>
       </c>
       <c r="P1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" t="s">
+        <v>188</v>
+      </c>
+      <c r="S1" t="s">
+        <v>189</v>
+      </c>
+      <c r="T1" t="s">
         <v>178</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>55</v>
       </c>
@@ -1560,11 +1600,23 @@
       <c r="O2" t="s">
         <v>147</v>
       </c>
-      <c r="Q2">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>187</v>
+      </c>
+      <c r="R2" t="s">
+        <v>190</v>
+      </c>
+      <c r="S2" t="s">
+        <v>191</v>
+      </c>
+      <c r="U2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>55</v>
       </c>
@@ -1610,11 +1662,23 @@
       <c r="O3" t="s">
         <v>147</v>
       </c>
-      <c r="Q3">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>187</v>
+      </c>
+      <c r="R3" t="s">
+        <v>190</v>
+      </c>
+      <c r="S3" t="s">
+        <v>191</v>
+      </c>
+      <c r="U3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>55</v>
       </c>
@@ -1660,11 +1724,23 @@
       <c r="O4" t="s">
         <v>147</v>
       </c>
-      <c r="Q4">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>187</v>
+      </c>
+      <c r="R4" t="s">
+        <v>190</v>
+      </c>
+      <c r="S4" t="s">
+        <v>191</v>
+      </c>
+      <c r="U4">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>55</v>
       </c>
@@ -1710,11 +1786,23 @@
       <c r="O5" t="s">
         <v>147</v>
       </c>
-      <c r="Q5">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>187</v>
+      </c>
+      <c r="R5" t="s">
+        <v>190</v>
+      </c>
+      <c r="S5" t="s">
+        <v>191</v>
+      </c>
+      <c r="U5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>55</v>
       </c>
@@ -1760,11 +1848,23 @@
       <c r="O6" t="s">
         <v>147</v>
       </c>
-      <c r="Q6">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>187</v>
+      </c>
+      <c r="R6" t="s">
+        <v>190</v>
+      </c>
+      <c r="S6" t="s">
+        <v>191</v>
+      </c>
+      <c r="U6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>55</v>
       </c>
@@ -1810,11 +1910,23 @@
       <c r="O7" t="s">
         <v>147</v>
       </c>
-      <c r="Q7">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>187</v>
+      </c>
+      <c r="R7" t="s">
+        <v>190</v>
+      </c>
+      <c r="S7" t="s">
+        <v>191</v>
+      </c>
+      <c r="U7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>55</v>
       </c>
@@ -1860,11 +1972,23 @@
       <c r="O8" t="s">
         <v>147</v>
       </c>
-      <c r="Q8">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>187</v>
+      </c>
+      <c r="R8" t="s">
+        <v>190</v>
+      </c>
+      <c r="S8" t="s">
+        <v>191</v>
+      </c>
+      <c r="U8">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>55</v>
       </c>
@@ -1910,11 +2034,23 @@
       <c r="O9" t="s">
         <v>147</v>
       </c>
-      <c r="Q9">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>187</v>
+      </c>
+      <c r="R9" t="s">
+        <v>190</v>
+      </c>
+      <c r="S9" t="s">
+        <v>191</v>
+      </c>
+      <c r="U9">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>55</v>
       </c>
@@ -1960,11 +2096,23 @@
       <c r="O10" t="s">
         <v>147</v>
       </c>
-      <c r="Q10">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>187</v>
+      </c>
+      <c r="R10" t="s">
+        <v>190</v>
+      </c>
+      <c r="S10" t="s">
+        <v>191</v>
+      </c>
+      <c r="U10">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>55</v>
       </c>
@@ -2010,11 +2158,23 @@
       <c r="O11" t="s">
         <v>147</v>
       </c>
-      <c r="Q11">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>187</v>
+      </c>
+      <c r="R11" t="s">
+        <v>190</v>
+      </c>
+      <c r="S11" t="s">
+        <v>191</v>
+      </c>
+      <c r="U11">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>55</v>
       </c>
@@ -2060,11 +2220,23 @@
       <c r="O12" t="s">
         <v>147</v>
       </c>
-      <c r="Q12">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>187</v>
+      </c>
+      <c r="R12" t="s">
+        <v>190</v>
+      </c>
+      <c r="S12" t="s">
+        <v>191</v>
+      </c>
+      <c r="U12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -2110,11 +2282,23 @@
       <c r="O13" t="s">
         <v>147</v>
       </c>
-      <c r="Q13">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>187</v>
+      </c>
+      <c r="R13" t="s">
+        <v>190</v>
+      </c>
+      <c r="S13" t="s">
+        <v>191</v>
+      </c>
+      <c r="U13">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>55</v>
       </c>
@@ -2160,11 +2344,23 @@
       <c r="O14" t="s">
         <v>147</v>
       </c>
-      <c r="Q14">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>187</v>
+      </c>
+      <c r="R14" t="s">
+        <v>190</v>
+      </c>
+      <c r="S14" t="s">
+        <v>191</v>
+      </c>
+      <c r="U14">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>55</v>
       </c>
@@ -2210,11 +2406,23 @@
       <c r="O15" t="s">
         <v>147</v>
       </c>
-      <c r="Q15">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>187</v>
+      </c>
+      <c r="R15" t="s">
+        <v>190</v>
+      </c>
+      <c r="S15" t="s">
+        <v>191</v>
+      </c>
+      <c r="U15">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>55</v>
       </c>
@@ -2260,11 +2468,23 @@
       <c r="O16" t="s">
         <v>147</v>
       </c>
-      <c r="Q16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>187</v>
+      </c>
+      <c r="R16" t="s">
+        <v>190</v>
+      </c>
+      <c r="S16" t="s">
+        <v>191</v>
+      </c>
+      <c r="U16">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>55</v>
       </c>
@@ -2310,11 +2530,23 @@
       <c r="O17" t="s">
         <v>147</v>
       </c>
-      <c r="Q17">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>187</v>
+      </c>
+      <c r="R17" t="s">
+        <v>190</v>
+      </c>
+      <c r="S17" t="s">
+        <v>191</v>
+      </c>
+      <c r="U17">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>55</v>
       </c>
@@ -2360,11 +2592,23 @@
       <c r="O18" t="s">
         <v>147</v>
       </c>
-      <c r="Q18">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>187</v>
+      </c>
+      <c r="R18" t="s">
+        <v>190</v>
+      </c>
+      <c r="S18" t="s">
+        <v>191</v>
+      </c>
+      <c r="U18">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>55</v>
       </c>
@@ -2410,11 +2654,23 @@
       <c r="O19" t="s">
         <v>147</v>
       </c>
-      <c r="Q19">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>187</v>
+      </c>
+      <c r="R19" t="s">
+        <v>190</v>
+      </c>
+      <c r="S19" t="s">
+        <v>191</v>
+      </c>
+      <c r="U19">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>55</v>
       </c>
@@ -2460,11 +2716,23 @@
       <c r="O20" t="s">
         <v>147</v>
       </c>
-      <c r="Q20">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>187</v>
+      </c>
+      <c r="R20" t="s">
+        <v>190</v>
+      </c>
+      <c r="S20" t="s">
+        <v>191</v>
+      </c>
+      <c r="U20">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>55</v>
       </c>
@@ -2510,11 +2778,23 @@
       <c r="O21" t="s">
         <v>147</v>
       </c>
-      <c r="Q21">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>187</v>
+      </c>
+      <c r="R21" t="s">
+        <v>190</v>
+      </c>
+      <c r="S21" t="s">
+        <v>191</v>
+      </c>
+      <c r="U21">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>55</v>
       </c>
@@ -2560,11 +2840,23 @@
       <c r="O22" t="s">
         <v>147</v>
       </c>
-      <c r="Q22">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>187</v>
+      </c>
+      <c r="R22" t="s">
+        <v>190</v>
+      </c>
+      <c r="S22" t="s">
+        <v>191</v>
+      </c>
+      <c r="U22">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>55</v>
       </c>
@@ -2610,11 +2902,23 @@
       <c r="O23" t="s">
         <v>147</v>
       </c>
-      <c r="Q23">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>187</v>
+      </c>
+      <c r="R23" t="s">
+        <v>190</v>
+      </c>
+      <c r="S23" t="s">
+        <v>191</v>
+      </c>
+      <c r="U23">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>55</v>
       </c>
@@ -2660,11 +2964,23 @@
       <c r="O24" t="s">
         <v>147</v>
       </c>
-      <c r="Q24">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>187</v>
+      </c>
+      <c r="R24" t="s">
+        <v>190</v>
+      </c>
+      <c r="S24" t="s">
+        <v>191</v>
+      </c>
+      <c r="U24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>55</v>
       </c>
@@ -2710,11 +3026,23 @@
       <c r="O25" t="s">
         <v>147</v>
       </c>
-      <c r="Q25">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>187</v>
+      </c>
+      <c r="R25" t="s">
+        <v>190</v>
+      </c>
+      <c r="S25" t="s">
+        <v>191</v>
+      </c>
+      <c r="U25">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>55</v>
       </c>
@@ -2760,11 +3088,23 @@
       <c r="O26" t="s">
         <v>147</v>
       </c>
-      <c r="Q26">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>187</v>
+      </c>
+      <c r="R26" t="s">
+        <v>190</v>
+      </c>
+      <c r="S26" t="s">
+        <v>191</v>
+      </c>
+      <c r="U26">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>55</v>
       </c>
@@ -2810,11 +3150,23 @@
       <c r="O27" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q27">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>187</v>
+      </c>
+      <c r="R27" t="s">
+        <v>190</v>
+      </c>
+      <c r="S27" t="s">
+        <v>191</v>
+      </c>
+      <c r="U27">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>55</v>
       </c>
@@ -2860,11 +3212,23 @@
       <c r="O28" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q28">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P28" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>187</v>
+      </c>
+      <c r="R28" t="s">
+        <v>190</v>
+      </c>
+      <c r="S28" t="s">
+        <v>191</v>
+      </c>
+      <c r="U28">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>55</v>
       </c>
@@ -2910,11 +3274,23 @@
       <c r="O29" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q29">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>187</v>
+      </c>
+      <c r="R29" t="s">
+        <v>190</v>
+      </c>
+      <c r="S29" t="s">
+        <v>191</v>
+      </c>
+      <c r="U29">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>55</v>
       </c>
@@ -2960,11 +3336,23 @@
       <c r="O30" t="s">
         <v>147</v>
       </c>
-      <c r="Q30">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>187</v>
+      </c>
+      <c r="R30" t="s">
+        <v>190</v>
+      </c>
+      <c r="S30" t="s">
+        <v>191</v>
+      </c>
+      <c r="U30">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>55</v>
       </c>
@@ -3010,12 +3398,24 @@
       <c r="O31" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P31" s="2"/>
-      <c r="Q31">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>187</v>
+      </c>
+      <c r="R31" t="s">
+        <v>190</v>
+      </c>
+      <c r="S31" t="s">
+        <v>191</v>
+      </c>
+      <c r="T31" s="2"/>
+      <c r="U31">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>55</v>
       </c>
@@ -3061,11 +3461,23 @@
       <c r="O32" t="s">
         <v>147</v>
       </c>
-      <c r="Q32">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>187</v>
+      </c>
+      <c r="R32" t="s">
+        <v>190</v>
+      </c>
+      <c r="S32" t="s">
+        <v>191</v>
+      </c>
+      <c r="U32">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>55</v>
       </c>
@@ -3111,12 +3523,24 @@
       <c r="O33" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P33" s="2"/>
-      <c r="Q33">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>187</v>
+      </c>
+      <c r="R33" t="s">
+        <v>190</v>
+      </c>
+      <c r="S33" t="s">
+        <v>191</v>
+      </c>
+      <c r="T33" s="2"/>
+      <c r="U33">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>55</v>
       </c>
@@ -3162,11 +3586,23 @@
       <c r="O34" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q34">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>187</v>
+      </c>
+      <c r="R34" t="s">
+        <v>190</v>
+      </c>
+      <c r="S34" t="s">
+        <v>191</v>
+      </c>
+      <c r="U34">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>55</v>
       </c>
@@ -3212,11 +3648,23 @@
       <c r="O35" t="s">
         <v>147</v>
       </c>
-      <c r="Q35">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P35" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>187</v>
+      </c>
+      <c r="R35" t="s">
+        <v>190</v>
+      </c>
+      <c r="S35" t="s">
+        <v>191</v>
+      </c>
+      <c r="U35">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>55</v>
       </c>
@@ -3262,11 +3710,23 @@
       <c r="O36" t="s">
         <v>147</v>
       </c>
-      <c r="Q36">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>187</v>
+      </c>
+      <c r="R36" t="s">
+        <v>190</v>
+      </c>
+      <c r="S36" t="s">
+        <v>191</v>
+      </c>
+      <c r="U36">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>55</v>
       </c>
@@ -3312,11 +3772,23 @@
       <c r="O37" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q37">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P37" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>187</v>
+      </c>
+      <c r="R37" t="s">
+        <v>190</v>
+      </c>
+      <c r="S37" t="s">
+        <v>191</v>
+      </c>
+      <c r="U37">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>55</v>
       </c>
@@ -3362,11 +3834,23 @@
       <c r="O38" t="s">
         <v>147</v>
       </c>
-      <c r="Q38">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>187</v>
+      </c>
+      <c r="R38" t="s">
+        <v>190</v>
+      </c>
+      <c r="S38" t="s">
+        <v>191</v>
+      </c>
+      <c r="U38">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>55</v>
       </c>
@@ -3412,11 +3896,23 @@
       <c r="O39" t="s">
         <v>147</v>
       </c>
-      <c r="Q39">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>187</v>
+      </c>
+      <c r="R39" t="s">
+        <v>190</v>
+      </c>
+      <c r="S39" t="s">
+        <v>191</v>
+      </c>
+      <c r="U39">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>55</v>
       </c>
@@ -3462,11 +3958,23 @@
       <c r="O40" t="s">
         <v>147</v>
       </c>
-      <c r="Q40">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>187</v>
+      </c>
+      <c r="R40" t="s">
+        <v>190</v>
+      </c>
+      <c r="S40" t="s">
+        <v>191</v>
+      </c>
+      <c r="U40">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>55</v>
       </c>
@@ -3513,13 +4021,25 @@
         <v>147</v>
       </c>
       <c r="P41" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>187</v>
+      </c>
+      <c r="R41" t="s">
+        <v>190</v>
+      </c>
+      <c r="S41" t="s">
+        <v>191</v>
+      </c>
+      <c r="T41" t="s">
         <v>164</v>
       </c>
-      <c r="Q41">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U41">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>55</v>
       </c>
@@ -3565,11 +4085,23 @@
       <c r="O42" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q42">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P42" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>187</v>
+      </c>
+      <c r="R42" t="s">
+        <v>190</v>
+      </c>
+      <c r="S42" t="s">
+        <v>191</v>
+      </c>
+      <c r="U42">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>55</v>
       </c>
@@ -3616,13 +4148,25 @@
         <v>147</v>
       </c>
       <c r="P43" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>187</v>
+      </c>
+      <c r="R43" t="s">
+        <v>190</v>
+      </c>
+      <c r="S43" t="s">
+        <v>191</v>
+      </c>
+      <c r="T43" t="s">
         <v>159</v>
       </c>
-      <c r="Q43">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U43">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>55</v>
       </c>
@@ -3668,11 +4212,23 @@
       <c r="O44" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q44">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P44" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>187</v>
+      </c>
+      <c r="R44" t="s">
+        <v>190</v>
+      </c>
+      <c r="S44" t="s">
+        <v>191</v>
+      </c>
+      <c r="U44">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>55</v>
       </c>
@@ -3718,11 +4274,23 @@
       <c r="O45" t="s">
         <v>147</v>
       </c>
-      <c r="Q45">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P45" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>187</v>
+      </c>
+      <c r="R45" t="s">
+        <v>190</v>
+      </c>
+      <c r="S45" t="s">
+        <v>191</v>
+      </c>
+      <c r="U45">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>55</v>
       </c>
@@ -3768,11 +4336,23 @@
       <c r="O46" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q46">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P46" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>187</v>
+      </c>
+      <c r="R46" t="s">
+        <v>190</v>
+      </c>
+      <c r="S46" t="s">
+        <v>191</v>
+      </c>
+      <c r="U46">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>55</v>
       </c>
@@ -3819,13 +4399,25 @@
         <v>147</v>
       </c>
       <c r="P47" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>187</v>
+      </c>
+      <c r="R47" t="s">
+        <v>190</v>
+      </c>
+      <c r="S47" t="s">
+        <v>191</v>
+      </c>
+      <c r="T47" t="s">
         <v>156</v>
       </c>
-      <c r="Q47">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U47">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>55</v>
       </c>
@@ -3871,11 +4463,23 @@
       <c r="O48" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q48">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P48" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>187</v>
+      </c>
+      <c r="R48" t="s">
+        <v>190</v>
+      </c>
+      <c r="S48" t="s">
+        <v>191</v>
+      </c>
+      <c r="U48">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>55</v>
       </c>
@@ -3921,11 +4525,23 @@
       <c r="O49" t="s">
         <v>147</v>
       </c>
-      <c r="Q49">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P49" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>187</v>
+      </c>
+      <c r="R49" t="s">
+        <v>190</v>
+      </c>
+      <c r="S49" t="s">
+        <v>191</v>
+      </c>
+      <c r="U49">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>55</v>
       </c>
@@ -3971,12 +4587,24 @@
       <c r="O50" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P50" s="2"/>
-      <c r="Q50">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P50" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>187</v>
+      </c>
+      <c r="R50" t="s">
+        <v>190</v>
+      </c>
+      <c r="S50" t="s">
+        <v>191</v>
+      </c>
+      <c r="T50" s="2"/>
+      <c r="U50">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>55</v>
       </c>
@@ -4023,13 +4651,25 @@
         <v>147</v>
       </c>
       <c r="P51" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>187</v>
+      </c>
+      <c r="R51" t="s">
+        <v>190</v>
+      </c>
+      <c r="S51" t="s">
+        <v>191</v>
+      </c>
+      <c r="T51" t="s">
         <v>160</v>
       </c>
-      <c r="Q51">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U51">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>55</v>
       </c>
@@ -4075,12 +4715,24 @@
       <c r="O52" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P52" s="2"/>
-      <c r="Q52">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P52" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>187</v>
+      </c>
+      <c r="R52" t="s">
+        <v>190</v>
+      </c>
+      <c r="S52" t="s">
+        <v>191</v>
+      </c>
+      <c r="T52" s="2"/>
+      <c r="U52">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>55</v>
       </c>
@@ -4126,11 +4778,23 @@
       <c r="O53" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q53">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P53" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>187</v>
+      </c>
+      <c r="R53" t="s">
+        <v>190</v>
+      </c>
+      <c r="S53" t="s">
+        <v>191</v>
+      </c>
+      <c r="U53">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>55</v>
       </c>
@@ -4177,13 +4841,25 @@
         <v>147</v>
       </c>
       <c r="P54" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>187</v>
+      </c>
+      <c r="R54" t="s">
+        <v>190</v>
+      </c>
+      <c r="S54" t="s">
+        <v>191</v>
+      </c>
+      <c r="T54" t="s">
         <v>160</v>
       </c>
-      <c r="Q54">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U54">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>55</v>
       </c>
@@ -4230,13 +4906,25 @@
         <v>147</v>
       </c>
       <c r="P55" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>187</v>
+      </c>
+      <c r="R55" t="s">
+        <v>190</v>
+      </c>
+      <c r="S55" t="s">
+        <v>191</v>
+      </c>
+      <c r="T55" t="s">
         <v>158</v>
       </c>
-      <c r="Q55">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U55">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4283,13 +4971,25 @@
         <v>147</v>
       </c>
       <c r="P56" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>187</v>
+      </c>
+      <c r="R56" t="s">
+        <v>190</v>
+      </c>
+      <c r="S56" t="s">
+        <v>191</v>
+      </c>
+      <c r="T56" t="s">
         <v>157</v>
       </c>
-      <c r="Q56">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U56">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4335,11 +5035,23 @@
       <c r="O57" t="s">
         <v>147</v>
       </c>
-      <c r="Q57">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>187</v>
+      </c>
+      <c r="R57" t="s">
+        <v>190</v>
+      </c>
+      <c r="S57" t="s">
+        <v>191</v>
+      </c>
+      <c r="U57">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -4386,13 +5098,25 @@
         <v>147</v>
       </c>
       <c r="P58" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>187</v>
+      </c>
+      <c r="R58" t="s">
+        <v>190</v>
+      </c>
+      <c r="S58" t="s">
+        <v>191</v>
+      </c>
+      <c r="T58" t="s">
         <v>154</v>
       </c>
-      <c r="Q58">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U58">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>55</v>
       </c>
@@ -4438,11 +5162,23 @@
       <c r="O59" t="s">
         <v>147</v>
       </c>
-      <c r="Q59">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P59" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>187</v>
+      </c>
+      <c r="R59" t="s">
+        <v>190</v>
+      </c>
+      <c r="S59" t="s">
+        <v>191</v>
+      </c>
+      <c r="U59">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>55</v>
       </c>
@@ -4489,13 +5225,25 @@
         <v>147</v>
       </c>
       <c r="P60" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>187</v>
+      </c>
+      <c r="R60" t="s">
+        <v>190</v>
+      </c>
+      <c r="S60" t="s">
+        <v>191</v>
+      </c>
+      <c r="T60" t="s">
         <v>169</v>
       </c>
-      <c r="Q60">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U60">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>55</v>
       </c>
@@ -4542,13 +5290,25 @@
         <v>147</v>
       </c>
       <c r="P61" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>187</v>
+      </c>
+      <c r="R61" t="s">
+        <v>190</v>
+      </c>
+      <c r="S61" t="s">
+        <v>191</v>
+      </c>
+      <c r="T61" t="s">
         <v>153</v>
       </c>
-      <c r="Q61">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U61">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>55</v>
       </c>
@@ -4595,13 +5355,25 @@
         <v>147</v>
       </c>
       <c r="P62" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>187</v>
+      </c>
+      <c r="R62" t="s">
+        <v>190</v>
+      </c>
+      <c r="S62" t="s">
+        <v>191</v>
+      </c>
+      <c r="T62" t="s">
         <v>154</v>
       </c>
-      <c r="Q62">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U62">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>55</v>
       </c>
@@ -4648,13 +5420,25 @@
         <v>147</v>
       </c>
       <c r="P63" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>187</v>
+      </c>
+      <c r="R63" t="s">
+        <v>190</v>
+      </c>
+      <c r="S63" t="s">
+        <v>191</v>
+      </c>
+      <c r="T63" t="s">
         <v>168</v>
       </c>
-      <c r="Q63">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U63">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>55</v>
       </c>
@@ -4700,11 +5484,23 @@
       <c r="O64" t="s">
         <v>147</v>
       </c>
-      <c r="Q64">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P64" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>187</v>
+      </c>
+      <c r="R64" t="s">
+        <v>190</v>
+      </c>
+      <c r="S64" t="s">
+        <v>191</v>
+      </c>
+      <c r="U64">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>55</v>
       </c>
@@ -4750,11 +5546,23 @@
       <c r="O65" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q65">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>187</v>
+      </c>
+      <c r="R65" t="s">
+        <v>190</v>
+      </c>
+      <c r="S65" t="s">
+        <v>191</v>
+      </c>
+      <c r="U65">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>55</v>
       </c>
@@ -4800,11 +5608,23 @@
       <c r="O66" t="s">
         <v>147</v>
       </c>
-      <c r="Q66">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P66" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>187</v>
+      </c>
+      <c r="R66" t="s">
+        <v>190</v>
+      </c>
+      <c r="S66" t="s">
+        <v>191</v>
+      </c>
+      <c r="U66">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>55</v>
       </c>
@@ -4850,12 +5670,24 @@
       <c r="O67" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P67" s="2"/>
-      <c r="Q67">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P67" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>187</v>
+      </c>
+      <c r="R67" t="s">
+        <v>190</v>
+      </c>
+      <c r="S67" t="s">
+        <v>191</v>
+      </c>
+      <c r="T67" s="2"/>
+      <c r="U67">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>55</v>
       </c>
@@ -4902,13 +5734,25 @@
         <v>147</v>
       </c>
       <c r="P68" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>187</v>
+      </c>
+      <c r="R68" t="s">
+        <v>190</v>
+      </c>
+      <c r="S68" t="s">
+        <v>191</v>
+      </c>
+      <c r="T68" t="s">
         <v>160</v>
       </c>
-      <c r="Q68">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U68">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>55</v>
       </c>
@@ -4954,11 +5798,23 @@
       <c r="O69" t="s">
         <v>147</v>
       </c>
-      <c r="Q69">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P69" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>187</v>
+      </c>
+      <c r="R69" t="s">
+        <v>190</v>
+      </c>
+      <c r="S69" t="s">
+        <v>191</v>
+      </c>
+      <c r="U69">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>55</v>
       </c>
@@ -5004,11 +5860,23 @@
       <c r="O70" t="s">
         <v>147</v>
       </c>
-      <c r="Q70">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P70" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>187</v>
+      </c>
+      <c r="R70" t="s">
+        <v>190</v>
+      </c>
+      <c r="S70" t="s">
+        <v>191</v>
+      </c>
+      <c r="U70">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>55</v>
       </c>
@@ -5055,13 +5923,25 @@
         <v>147</v>
       </c>
       <c r="P71" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>187</v>
+      </c>
+      <c r="R71" t="s">
+        <v>190</v>
+      </c>
+      <c r="S71" t="s">
+        <v>191</v>
+      </c>
+      <c r="T71" t="s">
         <v>154</v>
       </c>
-      <c r="Q71">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U71">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>55</v>
       </c>
@@ -5108,13 +5988,25 @@
         <v>147</v>
       </c>
       <c r="P72" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>187</v>
+      </c>
+      <c r="R72" t="s">
+        <v>190</v>
+      </c>
+      <c r="S72" t="s">
+        <v>191</v>
+      </c>
+      <c r="T72" t="s">
         <v>168</v>
       </c>
-      <c r="Q72">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U72">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>55</v>
       </c>
@@ -5161,13 +6053,25 @@
         <v>147</v>
       </c>
       <c r="P73" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>187</v>
+      </c>
+      <c r="R73" t="s">
+        <v>190</v>
+      </c>
+      <c r="S73" t="s">
+        <v>191</v>
+      </c>
+      <c r="T73" t="s">
         <v>154</v>
       </c>
-      <c r="Q73">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U73">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>55</v>
       </c>
@@ -5214,13 +6118,25 @@
         <v>147</v>
       </c>
       <c r="P74" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>187</v>
+      </c>
+      <c r="R74" t="s">
+        <v>190</v>
+      </c>
+      <c r="S74" t="s">
+        <v>191</v>
+      </c>
+      <c r="T74" t="s">
         <v>154</v>
       </c>
-      <c r="Q74">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U74">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>55</v>
       </c>
@@ -5266,12 +6182,24 @@
       <c r="O75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P75" s="2"/>
-      <c r="Q75">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P75" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>187</v>
+      </c>
+      <c r="R75" t="s">
+        <v>190</v>
+      </c>
+      <c r="S75" t="s">
+        <v>191</v>
+      </c>
+      <c r="T75" s="2"/>
+      <c r="U75">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>55</v>
       </c>
@@ -5317,11 +6245,23 @@
       <c r="O76" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q76">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P76" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>187</v>
+      </c>
+      <c r="R76" t="s">
+        <v>190</v>
+      </c>
+      <c r="S76" t="s">
+        <v>191</v>
+      </c>
+      <c r="U76">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>55</v>
       </c>
@@ -5367,12 +6307,24 @@
       <c r="O77" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P77" s="2"/>
-      <c r="Q77">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P77" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>187</v>
+      </c>
+      <c r="R77" t="s">
+        <v>190</v>
+      </c>
+      <c r="S77" t="s">
+        <v>191</v>
+      </c>
+      <c r="T77" s="2"/>
+      <c r="U77">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>55</v>
       </c>
@@ -5419,13 +6371,25 @@
         <v>147</v>
       </c>
       <c r="P78" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>187</v>
+      </c>
+      <c r="R78" t="s">
+        <v>190</v>
+      </c>
+      <c r="S78" t="s">
+        <v>191</v>
+      </c>
+      <c r="T78" t="s">
         <v>155</v>
       </c>
-      <c r="Q78">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U78">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>55</v>
       </c>
@@ -5472,13 +6436,25 @@
         <v>147</v>
       </c>
       <c r="P79" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>187</v>
+      </c>
+      <c r="R79" t="s">
+        <v>190</v>
+      </c>
+      <c r="S79" t="s">
+        <v>191</v>
+      </c>
+      <c r="T79" t="s">
         <v>165</v>
       </c>
-      <c r="Q79">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U79">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>55</v>
       </c>
@@ -5524,11 +6500,23 @@
       <c r="O80" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q80">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P80" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>187</v>
+      </c>
+      <c r="R80" t="s">
+        <v>190</v>
+      </c>
+      <c r="S80" t="s">
+        <v>191</v>
+      </c>
+      <c r="U80">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>55</v>
       </c>
@@ -5575,13 +6563,25 @@
         <v>147</v>
       </c>
       <c r="P81" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>187</v>
+      </c>
+      <c r="R81" t="s">
+        <v>190</v>
+      </c>
+      <c r="S81" t="s">
+        <v>191</v>
+      </c>
+      <c r="T81" t="s">
         <v>154</v>
       </c>
-      <c r="Q81">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U81">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>55</v>
       </c>
@@ -5627,11 +6627,23 @@
       <c r="O82" t="s">
         <v>147</v>
       </c>
-      <c r="Q82">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P82" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>187</v>
+      </c>
+      <c r="R82" t="s">
+        <v>190</v>
+      </c>
+      <c r="S82" t="s">
+        <v>191</v>
+      </c>
+      <c r="U82">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>55</v>
       </c>
@@ -5678,13 +6690,25 @@
         <v>147</v>
       </c>
       <c r="P83" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>187</v>
+      </c>
+      <c r="R83" t="s">
+        <v>190</v>
+      </c>
+      <c r="S83" t="s">
+        <v>191</v>
+      </c>
+      <c r="T83" t="s">
         <v>171</v>
       </c>
-      <c r="Q83">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U83">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>55</v>
       </c>
@@ -5731,13 +6755,25 @@
         <v>147</v>
       </c>
       <c r="P84" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>187</v>
+      </c>
+      <c r="R84" t="s">
+        <v>190</v>
+      </c>
+      <c r="S84" t="s">
+        <v>191</v>
+      </c>
+      <c r="T84" t="s">
         <v>168</v>
       </c>
-      <c r="Q84">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U84">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>55</v>
       </c>
@@ -5783,11 +6819,23 @@
       <c r="O85" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q85">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P85" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>187</v>
+      </c>
+      <c r="R85" t="s">
+        <v>190</v>
+      </c>
+      <c r="S85" t="s">
+        <v>191</v>
+      </c>
+      <c r="U85">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>55</v>
       </c>
@@ -5834,13 +6882,25 @@
         <v>147</v>
       </c>
       <c r="P86" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>187</v>
+      </c>
+      <c r="R86" t="s">
+        <v>190</v>
+      </c>
+      <c r="S86" t="s">
+        <v>191</v>
+      </c>
+      <c r="T86" t="s">
         <v>168</v>
       </c>
-      <c r="Q86">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U86">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>55</v>
       </c>
@@ -5887,13 +6947,25 @@
         <v>147</v>
       </c>
       <c r="P87" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>187</v>
+      </c>
+      <c r="R87" t="s">
+        <v>190</v>
+      </c>
+      <c r="S87" t="s">
+        <v>191</v>
+      </c>
+      <c r="T87" t="s">
         <v>161</v>
       </c>
-      <c r="Q87">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U87">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>55</v>
       </c>
@@ -5939,12 +7011,24 @@
       <c r="O88" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P88" s="2"/>
-      <c r="Q88">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P88" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>187</v>
+      </c>
+      <c r="R88" t="s">
+        <v>190</v>
+      </c>
+      <c r="S88" t="s">
+        <v>191</v>
+      </c>
+      <c r="T88" s="2"/>
+      <c r="U88">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>55</v>
       </c>
@@ -5991,13 +7075,25 @@
         <v>147</v>
       </c>
       <c r="P89" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>187</v>
+      </c>
+      <c r="R89" t="s">
+        <v>190</v>
+      </c>
+      <c r="S89" t="s">
+        <v>191</v>
+      </c>
+      <c r="T89" t="s">
         <v>172</v>
       </c>
-      <c r="Q89">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U89">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>55</v>
       </c>
@@ -6043,12 +7139,24 @@
       <c r="O90" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P90" s="2"/>
-      <c r="Q90">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P90" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>187</v>
+      </c>
+      <c r="R90" t="s">
+        <v>190</v>
+      </c>
+      <c r="S90" t="s">
+        <v>191</v>
+      </c>
+      <c r="T90" s="2"/>
+      <c r="U90">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>55</v>
       </c>
@@ -6094,12 +7202,24 @@
       <c r="O91" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P91" s="2"/>
-      <c r="Q91">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P91" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>187</v>
+      </c>
+      <c r="R91" t="s">
+        <v>190</v>
+      </c>
+      <c r="S91" t="s">
+        <v>191</v>
+      </c>
+      <c r="T91" s="2"/>
+      <c r="U91">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>55</v>
       </c>
@@ -6146,13 +7266,25 @@
         <v>147</v>
       </c>
       <c r="P92" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>187</v>
+      </c>
+      <c r="R92" t="s">
+        <v>190</v>
+      </c>
+      <c r="S92" t="s">
+        <v>191</v>
+      </c>
+      <c r="T92" t="s">
         <v>167</v>
       </c>
-      <c r="Q92">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U92">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>55</v>
       </c>
@@ -6199,13 +7331,25 @@
         <v>147</v>
       </c>
       <c r="P93" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>187</v>
+      </c>
+      <c r="R93" t="s">
+        <v>190</v>
+      </c>
+      <c r="S93" t="s">
+        <v>191</v>
+      </c>
+      <c r="T93" t="s">
         <v>163</v>
       </c>
-      <c r="Q93">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U93">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>55</v>
       </c>
@@ -6251,11 +7395,23 @@
       <c r="O94" t="s">
         <v>147</v>
       </c>
-      <c r="Q94">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P94" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>187</v>
+      </c>
+      <c r="R94" t="s">
+        <v>190</v>
+      </c>
+      <c r="S94" t="s">
+        <v>191</v>
+      </c>
+      <c r="U94">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>55</v>
       </c>
@@ -6301,11 +7457,23 @@
       <c r="O95" t="s">
         <v>147</v>
       </c>
-      <c r="Q95">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P95" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>187</v>
+      </c>
+      <c r="R95" t="s">
+        <v>190</v>
+      </c>
+      <c r="S95" t="s">
+        <v>191</v>
+      </c>
+      <c r="U95">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>55</v>
       </c>
@@ -6352,13 +7520,25 @@
         <v>147</v>
       </c>
       <c r="P96" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>187</v>
+      </c>
+      <c r="R96" t="s">
+        <v>190</v>
+      </c>
+      <c r="S96" t="s">
+        <v>191</v>
+      </c>
+      <c r="T96" t="s">
         <v>168</v>
       </c>
-      <c r="Q96">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U96">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>55</v>
       </c>
@@ -6405,13 +7585,25 @@
         <v>147</v>
       </c>
       <c r="P97" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>187</v>
+      </c>
+      <c r="R97" t="s">
+        <v>190</v>
+      </c>
+      <c r="S97" t="s">
+        <v>191</v>
+      </c>
+      <c r="T97" t="s">
         <v>166</v>
       </c>
-      <c r="Q97">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U97">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>55</v>
       </c>
@@ -6457,11 +7649,23 @@
       <c r="O98" t="s">
         <v>147</v>
       </c>
-      <c r="Q98">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P98" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>187</v>
+      </c>
+      <c r="R98" t="s">
+        <v>190</v>
+      </c>
+      <c r="S98" t="s">
+        <v>191</v>
+      </c>
+      <c r="U98">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>55</v>
       </c>
@@ -6508,13 +7712,25 @@
         <v>147</v>
       </c>
       <c r="P99" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>187</v>
+      </c>
+      <c r="R99" t="s">
+        <v>190</v>
+      </c>
+      <c r="S99" t="s">
+        <v>191</v>
+      </c>
+      <c r="T99" t="s">
         <v>162</v>
       </c>
-      <c r="Q99">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U99">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>55</v>
       </c>
@@ -6561,13 +7777,25 @@
         <v>147</v>
       </c>
       <c r="P100" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>187</v>
+      </c>
+      <c r="R100" t="s">
+        <v>190</v>
+      </c>
+      <c r="S100" t="s">
+        <v>191</v>
+      </c>
+      <c r="T100" t="s">
         <v>168</v>
       </c>
-      <c r="Q100">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U100">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>55</v>
       </c>
@@ -6613,11 +7841,23 @@
       <c r="O101" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q101">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P101" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>187</v>
+      </c>
+      <c r="R101" t="s">
+        <v>190</v>
+      </c>
+      <c r="S101" t="s">
+        <v>191</v>
+      </c>
+      <c r="U101">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>55</v>
       </c>
@@ -6664,13 +7904,25 @@
         <v>147</v>
       </c>
       <c r="P102" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>187</v>
+      </c>
+      <c r="R102" t="s">
+        <v>190</v>
+      </c>
+      <c r="S102" t="s">
+        <v>191</v>
+      </c>
+      <c r="T102" t="s">
         <v>170</v>
       </c>
-      <c r="Q102">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U102">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>55</v>
       </c>
@@ -6716,11 +7968,23 @@
       <c r="O103" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Q103">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P103" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>187</v>
+      </c>
+      <c r="R103" t="s">
+        <v>190</v>
+      </c>
+      <c r="S103" t="s">
+        <v>191</v>
+      </c>
+      <c r="U103">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>55</v>
       </c>
@@ -6767,13 +8031,25 @@
         <v>149</v>
       </c>
       <c r="P104" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>187</v>
+      </c>
+      <c r="R104" t="s">
+        <v>190</v>
+      </c>
+      <c r="S104" t="s">
+        <v>191</v>
+      </c>
+      <c r="T104" t="s">
         <v>150</v>
       </c>
-      <c r="Q104">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U104">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>55</v>
       </c>
@@ -6820,13 +8096,25 @@
         <v>149</v>
       </c>
       <c r="P105" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>187</v>
+      </c>
+      <c r="R105" t="s">
+        <v>190</v>
+      </c>
+      <c r="S105" t="s">
+        <v>191</v>
+      </c>
+      <c r="T105" t="s">
         <v>174</v>
       </c>
-      <c r="Q105">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="U105">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>55</v>
       </c>
@@ -6873,14 +8161,26 @@
         <v>149</v>
       </c>
       <c r="P106" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>187</v>
+      </c>
+      <c r="R106" t="s">
+        <v>190</v>
+      </c>
+      <c r="S106" t="s">
+        <v>191</v>
+      </c>
+      <c r="T106" t="s">
         <v>173</v>
       </c>
-      <c r="Q106">
+      <c r="U106">
         <v>2019</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q106" xr:uid="{84F43E81-2022-4DFD-8A77-BA88645FF9B4}"/>
+  <autoFilter ref="A1:U106" xr:uid="{84F43E81-2022-4DFD-8A77-BA88645FF9B4}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>